<commit_message>
looting system 1차 완성
아직 안돌려봄
</commit_message>
<xml_diff>
--- a/Unity Project/Assets/Resources/Data/ItemData.xlsx
+++ b/Unity Project/Assets/Resources/Data/ItemData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\senier project\RRD\Unity Project\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351DBD19-ADD5-4A6D-B66D-C86027D304EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8490D8-CACE-48D2-BF82-2F4BC9F70106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24137" yWindow="3574" windowWidth="30720" windowHeight="12609" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23031" yWindow="3240" windowWidth="30720" windowHeight="12454" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemSheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>id</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>Legendry</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dropMonster</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Orc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goblin</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -447,7 +459,7 @@
     <col min="7" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="25.2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,10 +473,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -477,49 +492,70 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
         <v>4</v>
       </c>
     </row>

</xml_diff>